<commit_message>
Reading data from excel
Module: AppContent
Providing inputs to upload file through data provider by reading data
from excel sheet
</commit_message>
<xml_diff>
--- a/bin/com/excel/RegressionSuiteTestCases.xlsx
+++ b/bin/com/excel/RegressionSuiteTestCases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>./src/com/autoitfiles/upload_bmp.exe</t>
+  </si>
+  <si>
+    <t>./src/com/autoitfiles/upload_gif.exe</t>
+  </si>
+  <si>
+    <t>./src/com/autoitfiles/upload_jpeg.exe</t>
   </si>
 </sst>
 </file>
@@ -661,46 +667,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>